<commit_message>
Still problem 1 and 3
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="problem_1" sheetId="1" r:id="rId1"/>
     <sheet name="problem_3" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>loss</t>
   </si>
@@ -122,7 +123,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LSLC</c:v>
+                  <c:v>SVM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -215,64 +216,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1.5E-3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.5000000000000001E-3</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.5E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.5E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.5E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>1.5E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2E-3</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>3.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.4999999999999997E-3</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.4999999999999997E-3</c:v>
+                  <c:v>5.4999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>6.4999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.4999999999999998E-3</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.4999999999999998E-3</c:v>
+                  <c:v>1.0999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0500000000000001E-2</c:v>
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2500000000000001E-2</c:v>
+                  <c:v>2.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.7999999999999999E-2</c:v>
+                  <c:v>2.5499999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -525,7 +526,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LSLC</c:v>
+                  <c:v>SVM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -618,64 +619,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1.5E-3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.5000000000000001E-3</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.5E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.5E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>1.5E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>1.5E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2E-3</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>3.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5000000000000001E-3</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.4999999999999997E-3</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.4999999999999997E-3</c:v>
+                  <c:v>5.4999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>6.4999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.4999999999999998E-3</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.4999999999999998E-3</c:v>
+                  <c:v>1.0999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0500000000000001E-2</c:v>
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2500000000000001E-2</c:v>
+                  <c:v>2.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.7999999999999999E-2</c:v>
+                  <c:v>2.5499999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1253,124 +1254,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38666666666666699</c:v>
+                  <c:v>4.6666666666666697E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36499999999999999</c:v>
+                  <c:v>3.2500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35599999999999998</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.34666666666666701</c:v>
+                  <c:v>3.1666666666666697E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.33428571428571402</c:v>
+                  <c:v>3.7142857142857102E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.35</c:v>
+                  <c:v>3.2500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.335555555555556</c:v>
+                  <c:v>3.4444444444444403E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.34</c:v>
+                  <c:v>2.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.32909090909090899</c:v>
+                  <c:v>3.2727272727272702E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.32166666666666699</c:v>
+                  <c:v>2.4166666666666701E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.29384615384615398</c:v>
+                  <c:v>3.4615384615384603E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.26285714285714301</c:v>
+                  <c:v>2.78571428571429E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.266666666666667</c:v>
+                  <c:v>2.8666666666666701E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.26250000000000001</c:v>
+                  <c:v>3.9375E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.25647058823529401</c:v>
+                  <c:v>3.1764705882352903E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.26333333333333298</c:v>
+                  <c:v>2.8333333333333301E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.26</c:v>
+                  <c:v>2.2105263157894701E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.26</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.24666666666666701</c:v>
+                  <c:v>2.5238095238095198E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.25272727272727302</c:v>
+                  <c:v>2.68181818181818E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.24</c:v>
+                  <c:v>2.3913043478260902E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.236666666666667</c:v>
+                  <c:v>3.6666666666666702E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.2336</c:v>
+                  <c:v>4.3200000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.22307692307692301</c:v>
+                  <c:v>2.5384615384615401E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.21185185185185201</c:v>
+                  <c:v>4.2592592592592599E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.215714285714286</c:v>
+                  <c:v>3.3214285714285703E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.20827586206896601</c:v>
+                  <c:v>2.7931034482758601E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.204666666666667</c:v>
+                  <c:v>2.8666666666666701E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.21741935483871</c:v>
+                  <c:v>2.4838709677419399E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.20125000000000001</c:v>
+                  <c:v>2.8125000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.192121212121212</c:v>
+                  <c:v>2.4242424242424201E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.188823529411765</c:v>
+                  <c:v>2.32352941176471E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.188</c:v>
+                  <c:v>2.4285714285714299E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.2</c:v>
+                  <c:v>2.75E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.196756756756757</c:v>
+                  <c:v>2.59459459459459E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.19578947368421101</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.18974358974359001</c:v>
+                  <c:v>2.5384615384615401E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.1875</c:v>
+                  <c:v>3.2250000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1544,124 +1545,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>0.42</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34499999999999997</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35199999999999998</c:v>
+                  <c:v>0.35399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.37</c:v>
+                  <c:v>0.39333333333333298</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.33428571428571402</c:v>
+                  <c:v>0.39571428571428602</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.315</c:v>
+                  <c:v>0.505</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.32222222222222202</c:v>
+                  <c:v>0.301111111111111</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.32400000000000001</c:v>
+                  <c:v>0.28199999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.30545454545454598</c:v>
+                  <c:v>0.279090909090909</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.28499999999999998</c:v>
+                  <c:v>0.26833333333333298</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.25538461538461499</c:v>
+                  <c:v>0.265384615384615</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.252857142857143</c:v>
+                  <c:v>0.26142857142857101</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.29466666666666702</c:v>
+                  <c:v>0.26066666666666699</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.26624999999999999</c:v>
+                  <c:v>0.25874999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.223529411764706</c:v>
+                  <c:v>0.25588235294117601</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.21666666666666701</c:v>
+                  <c:v>0.25333333333333302</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.28947368421052599</c:v>
+                  <c:v>0.25421052631579</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.20799999999999999</c:v>
+                  <c:v>0.253</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.22380952380952401</c:v>
+                  <c:v>0.25190476190476202</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.20272727272727301</c:v>
+                  <c:v>0.25090909090909103</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.20956521739130399</c:v>
+                  <c:v>0.25086956521739101</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.211666666666667</c:v>
+                  <c:v>0.2525</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.22800000000000001</c:v>
+                  <c:v>0.25240000000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.23230769230769199</c:v>
+                  <c:v>0.25230769230769201</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.20444444444444401</c:v>
+                  <c:v>0.252962962962963</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.19714285714285701</c:v>
+                  <c:v>0.253571428571429</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.20206896551724099</c:v>
+                  <c:v>0.25413793103448301</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.19266666666666701</c:v>
+                  <c:v>0.25333333333333302</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.21290322580645199</c:v>
+                  <c:v>0.25451612903225801</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.20624999999999999</c:v>
+                  <c:v>0.255</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.18606060606060601</c:v>
+                  <c:v>0.25424242424242399</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.192352941176471</c:v>
+                  <c:v>0.252941176470588</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.23657142857142899</c:v>
+                  <c:v>0.253428571428571</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.19277777777777799</c:v>
+                  <c:v>0.253888888888889</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.19405405405405399</c:v>
+                  <c:v>0.25324324324324299</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.19578947368421101</c:v>
+                  <c:v>0.25263157894736799</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.20256410256410301</c:v>
+                  <c:v>0.25307692307692298</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.1895</c:v>
+                  <c:v>0.253</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1888,6 +1889,1428 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>problem_3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>problem_3!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1550</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>problem_3!$B$2:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6666666666666697E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1666666666666697E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.7142857142857102E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4444444444444403E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.2727272727272702E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4166666666666701E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.4615384615384603E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.78571428571429E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8666666666666701E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.9375E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.1764705882352903E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.8333333333333301E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.2105263157894701E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.5238095238095198E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.68181818181818E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.3913043478260902E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.6666666666666702E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.3200000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5384615384615401E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.2592592592592599E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.3214285714285703E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.7931034482758601E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.8666666666666701E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.4838709677419399E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.8125000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.4242424242424201E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.32352941176471E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.4285714285714299E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.75E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.59459459459459E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.5384615384615401E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.2250000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E494-43F0-90C2-769AD6E6F77C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>problem_3!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LSLC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>problem_3!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1550</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>problem_3!$C$2:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.39333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39571428571428602</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.505</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.301111111111111</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.279090909090909</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26833333333333298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.265384615384615</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26142857142857101</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26066666666666699</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25874999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25588235294117601</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25333333333333302</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.25421052631579</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.253</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.25190476190476202</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25090909090909103</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25086956521739101</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.2525</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.25240000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25230769230769201</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.252962962962963</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.253571428571429</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.25413793103448301</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.25333333333333302</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.25451612903225801</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.255</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.25424242424242399</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.252941176470588</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.253428571428571</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.253888888888889</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.25324324324324299</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.25263157894736799</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.25307692307692298</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.253</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E494-43F0-90C2-769AD6E6F77C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="525212504"/>
+        <c:axId val="525204632"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="525212504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="525204632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="525204632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.60000000000000009"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="525212504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.39333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.40400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.38666666666666699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.40285714285714302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.40250000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41777777777777803</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.41399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.40727272727272701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.418333333333333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.39692307692307699</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.398666666666667</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.40125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.41529411764705898</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.41222222222222199</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.35368421052631599</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0213-4029-93DC-0FE6B3119C6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LSLC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39714285714285702</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.41499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.43777777777777799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.41599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.45636363636363603</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.391666666666667</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.395384615384615</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.40285714285714302</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.38533333333333297</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.37874999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.42941176470588199</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.43888888888888899</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.35368421052631599</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.38900000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0213-4029-93DC-0FE6B3119C6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="441771328"/>
+        <c:axId val="441771984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="441771328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441771984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="441771984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="441771328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2008,6 +3431,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3556,20 +5059,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3590,13 +6125,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>4762</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>309562</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -3625,16 +6160,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>519112</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>214312</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>233362</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3648,6 +6183,73 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3921,8 +6523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3941,7 +6543,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -3959,7 +6561,7 @@
         <v>100000000</v>
       </c>
       <c r="D2">
-        <v>1.5E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="E2">
         <v>7.1999999999999995E-2</v>
@@ -3977,7 +6579,7 @@
         <v>33598182.862837799</v>
       </c>
       <c r="D3">
-        <v>2.5000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="E3">
         <v>7.1999999999999995E-2</v>
@@ -3995,7 +6597,7 @@
         <v>11288378.916846886</v>
       </c>
       <c r="D4">
-        <v>2E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="E4">
         <v>7.1999999999999995E-2</v>
@@ -4013,7 +6615,7 @@
         <v>3792690.1907322467</v>
       </c>
       <c r="D5">
-        <v>2E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="E5">
         <v>7.1999999999999995E-2</v>
@@ -4031,7 +6633,7 @@
         <v>1274274.9857031342</v>
       </c>
       <c r="D6">
-        <v>2.5000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="E6">
         <v>7.1999999999999995E-2</v>
@@ -4067,7 +6669,7 @@
         <v>143844.98882876622</v>
       </c>
       <c r="D8">
-        <v>3.0000000000000001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="E8">
         <v>7.1999999999999995E-2</v>
@@ -4085,7 +6687,7 @@
         <v>48329.302385717521</v>
       </c>
       <c r="D9">
-        <v>2E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="E9">
         <v>7.1999999999999995E-2</v>
@@ -4103,7 +6705,7 @@
         <v>16237.767391887226</v>
       </c>
       <c r="D10">
-        <v>2.5000000000000001E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="E10">
         <v>7.1999999999999995E-2</v>
@@ -4139,7 +6741,7 @@
         <v>1832.9807108324355</v>
       </c>
       <c r="D12">
-        <v>2.5000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E12">
         <v>7.1999999999999995E-2</v>
@@ -4157,7 +6759,7 @@
         <v>615.84821106602703</v>
       </c>
       <c r="D13">
-        <v>4.4999999999999997E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E13">
         <v>7.1999999999999995E-2</v>
@@ -4175,7 +6777,7 @@
         <v>206.91380811147911</v>
       </c>
       <c r="D14">
-        <v>5.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E14">
         <v>7.1999999999999995E-2</v>
@@ -4193,7 +6795,7 @@
         <v>69.519279617756197</v>
       </c>
       <c r="D15">
-        <v>6.4999999999999997E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="E15">
         <v>7.1999999999999995E-2</v>
@@ -4229,7 +6831,7 @@
         <v>7.8475997035146365</v>
       </c>
       <c r="D17">
-        <v>9.4999999999999998E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="E17">
         <v>7.1999999999999995E-2</v>
@@ -4247,7 +6849,7 @@
         <v>2.6366508987303581</v>
       </c>
       <c r="D18">
-        <v>9.4999999999999998E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="E18">
         <v>7.1999999999999995E-2</v>
@@ -4265,7 +6867,7 @@
         <v>0.88586679041008187</v>
       </c>
       <c r="D19">
-        <v>1.0500000000000001E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="E19">
         <v>7.1999999999999995E-2</v>
@@ -4283,7 +6885,7 @@
         <v>0.29763514416313108</v>
       </c>
       <c r="D20">
-        <v>1.2500000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="E20">
         <v>7.1999999999999995E-2</v>
@@ -4301,7 +6903,7 @@
         <v>0.1</v>
       </c>
       <c r="D21">
-        <v>1.7999999999999999E-2</v>
+        <v>2.5499999999999998E-2</v>
       </c>
       <c r="E21">
         <v>7.1999999999999995E-2</v>
@@ -4317,8 +6919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4339,10 +6941,10 @@
         <v>50</v>
       </c>
       <c r="B2">
-        <v>0.4</v>
+        <v>0.08</v>
       </c>
       <c r="C2">
-        <v>0.42</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4350,10 +6952,10 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>0.32</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C3">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4361,10 +6963,10 @@
         <v>150</v>
       </c>
       <c r="B4">
-        <v>0.38666666666666699</v>
+        <v>4.6666666666666697E-2</v>
       </c>
       <c r="C4">
-        <v>0.4</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4372,10 +6974,10 @@
         <v>200</v>
       </c>
       <c r="B5">
-        <v>0.36499999999999999</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="C5">
-        <v>0.34499999999999997</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4383,10 +6985,10 @@
         <v>250</v>
       </c>
       <c r="B6">
-        <v>0.35599999999999998</v>
+        <v>0.03</v>
       </c>
       <c r="C6">
-        <v>0.35199999999999998</v>
+        <v>0.35399999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -4394,10 +6996,10 @@
         <v>300</v>
       </c>
       <c r="B7">
-        <v>0.34666666666666701</v>
+        <v>3.1666666666666697E-2</v>
       </c>
       <c r="C7">
-        <v>0.37</v>
+        <v>0.39333333333333298</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4405,10 +7007,10 @@
         <v>350</v>
       </c>
       <c r="B8">
-        <v>0.33428571428571402</v>
+        <v>3.7142857142857102E-2</v>
       </c>
       <c r="C8">
-        <v>0.33428571428571402</v>
+        <v>0.39571428571428602</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4416,10 +7018,10 @@
         <v>400</v>
       </c>
       <c r="B9">
-        <v>0.35</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="C9">
-        <v>0.315</v>
+        <v>0.505</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4427,10 +7029,10 @@
         <v>450</v>
       </c>
       <c r="B10">
-        <v>0.335555555555556</v>
+        <v>3.4444444444444403E-2</v>
       </c>
       <c r="C10">
-        <v>0.32222222222222202</v>
+        <v>0.301111111111111</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -4438,10 +7040,10 @@
         <v>500</v>
       </c>
       <c r="B11">
-        <v>0.34</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="C11">
-        <v>0.32400000000000001</v>
+        <v>0.28199999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4449,10 +7051,10 @@
         <v>550</v>
       </c>
       <c r="B12">
-        <v>0.32909090909090899</v>
+        <v>3.2727272727272702E-2</v>
       </c>
       <c r="C12">
-        <v>0.30545454545454598</v>
+        <v>0.279090909090909</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -4460,10 +7062,10 @@
         <v>600</v>
       </c>
       <c r="B13">
-        <v>0.32166666666666699</v>
+        <v>2.4166666666666701E-2</v>
       </c>
       <c r="C13">
-        <v>0.28499999999999998</v>
+        <v>0.26833333333333298</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -4471,10 +7073,10 @@
         <v>650</v>
       </c>
       <c r="B14">
-        <v>0.29384615384615398</v>
+        <v>3.4615384615384603E-2</v>
       </c>
       <c r="C14">
-        <v>0.25538461538461499</v>
+        <v>0.265384615384615</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -4482,10 +7084,10 @@
         <v>700</v>
       </c>
       <c r="B15">
-        <v>0.26285714285714301</v>
+        <v>2.78571428571429E-2</v>
       </c>
       <c r="C15">
-        <v>0.252857142857143</v>
+        <v>0.26142857142857101</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -4493,10 +7095,10 @@
         <v>750</v>
       </c>
       <c r="B16">
-        <v>0.266666666666667</v>
+        <v>2.8666666666666701E-2</v>
       </c>
       <c r="C16">
-        <v>0.29466666666666702</v>
+        <v>0.26066666666666699</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4504,10 +7106,10 @@
         <v>800</v>
       </c>
       <c r="B17">
-        <v>0.26250000000000001</v>
+        <v>3.9375E-2</v>
       </c>
       <c r="C17">
-        <v>0.26624999999999999</v>
+        <v>0.25874999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -4515,10 +7117,10 @@
         <v>850</v>
       </c>
       <c r="B18">
-        <v>0.25647058823529401</v>
+        <v>3.1764705882352903E-2</v>
       </c>
       <c r="C18">
-        <v>0.223529411764706</v>
+        <v>0.25588235294117601</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -4526,10 +7128,10 @@
         <v>900</v>
       </c>
       <c r="B19">
-        <v>0.26333333333333298</v>
+        <v>2.8333333333333301E-2</v>
       </c>
       <c r="C19">
-        <v>0.21666666666666701</v>
+        <v>0.25333333333333302</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -4537,10 +7139,10 @@
         <v>950</v>
       </c>
       <c r="B20">
-        <v>0.26</v>
+        <v>2.2105263157894701E-2</v>
       </c>
       <c r="C20">
-        <v>0.28947368421052599</v>
+        <v>0.25421052631579</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -4548,10 +7150,477 @@
         <v>1000</v>
       </c>
       <c r="B21">
-        <v>0.26</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C21">
-        <v>0.20799999999999999</v>
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1050</v>
+      </c>
+      <c r="B22">
+        <v>2.5238095238095198E-2</v>
+      </c>
+      <c r="C22">
+        <v>0.25190476190476202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1100</v>
+      </c>
+      <c r="B23">
+        <v>2.68181818181818E-2</v>
+      </c>
+      <c r="C23">
+        <v>0.25090909090909103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1150</v>
+      </c>
+      <c r="B24">
+        <v>2.3913043478260902E-2</v>
+      </c>
+      <c r="C24">
+        <v>0.25086956521739101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1200</v>
+      </c>
+      <c r="B25">
+        <v>3.6666666666666702E-2</v>
+      </c>
+      <c r="C25">
+        <v>0.2525</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1250</v>
+      </c>
+      <c r="B26">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="C26">
+        <v>0.25240000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1300</v>
+      </c>
+      <c r="B27">
+        <v>2.5384615384615401E-2</v>
+      </c>
+      <c r="C27">
+        <v>0.25230769230769201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1350</v>
+      </c>
+      <c r="B28">
+        <v>4.2592592592592599E-2</v>
+      </c>
+      <c r="C28">
+        <v>0.252962962962963</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1400</v>
+      </c>
+      <c r="B29">
+        <v>3.3214285714285703E-2</v>
+      </c>
+      <c r="C29">
+        <v>0.253571428571429</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1450</v>
+      </c>
+      <c r="B30">
+        <v>2.7931034482758601E-2</v>
+      </c>
+      <c r="C30">
+        <v>0.25413793103448301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1500</v>
+      </c>
+      <c r="B31">
+        <v>2.8666666666666701E-2</v>
+      </c>
+      <c r="C31">
+        <v>0.25333333333333302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1550</v>
+      </c>
+      <c r="B32">
+        <v>2.4838709677419399E-2</v>
+      </c>
+      <c r="C32">
+        <v>0.25451612903225801</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1600</v>
+      </c>
+      <c r="B33">
+        <v>2.8125000000000001E-2</v>
+      </c>
+      <c r="C33">
+        <v>0.255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1650</v>
+      </c>
+      <c r="B34">
+        <v>2.4242424242424201E-2</v>
+      </c>
+      <c r="C34">
+        <v>0.25424242424242399</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1700</v>
+      </c>
+      <c r="B35">
+        <v>2.32352941176471E-2</v>
+      </c>
+      <c r="C35">
+        <v>0.252941176470588</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1750</v>
+      </c>
+      <c r="B36">
+        <v>2.4285714285714299E-2</v>
+      </c>
+      <c r="C36">
+        <v>0.253428571428571</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1800</v>
+      </c>
+      <c r="B37">
+        <v>2.75E-2</v>
+      </c>
+      <c r="C37">
+        <v>0.253888888888889</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1850</v>
+      </c>
+      <c r="B38">
+        <v>2.59459459459459E-2</v>
+      </c>
+      <c r="C38">
+        <v>0.25324324324324299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1900</v>
+      </c>
+      <c r="B39">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C39">
+        <v>0.25263157894736799</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1950</v>
+      </c>
+      <c r="B40">
+        <v>2.5384615384615401E-2</v>
+      </c>
+      <c r="C40">
+        <v>0.25307692307692298</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2000</v>
+      </c>
+      <c r="B41">
+        <v>3.2250000000000001E-2</v>
+      </c>
+      <c r="C41">
+        <v>0.253</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>0.36</v>
+      </c>
+      <c r="C2">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>0.37</v>
+      </c>
+      <c r="C3">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>150</v>
+      </c>
+      <c r="B4">
+        <v>0.39333333333333298</v>
+      </c>
+      <c r="C4">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>200</v>
+      </c>
+      <c r="B5">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="C5">
+        <v>0.45500000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>250</v>
+      </c>
+      <c r="B6">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="C6">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>300</v>
+      </c>
+      <c r="B7">
+        <v>0.38666666666666699</v>
+      </c>
+      <c r="C7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>350</v>
+      </c>
+      <c r="B8">
+        <v>0.40285714285714302</v>
+      </c>
+      <c r="C8">
+        <v>0.39714285714285702</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>400</v>
+      </c>
+      <c r="B9">
+        <v>0.40250000000000002</v>
+      </c>
+      <c r="C9">
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>450</v>
+      </c>
+      <c r="B10">
+        <v>0.41777777777777803</v>
+      </c>
+      <c r="C10">
+        <v>0.43777777777777799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>500</v>
+      </c>
+      <c r="B11">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="C11">
+        <v>0.41599999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>550</v>
+      </c>
+      <c r="B12">
+        <v>0.40727272727272701</v>
+      </c>
+      <c r="C12">
+        <v>0.45636363636363603</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>600</v>
+      </c>
+      <c r="B13">
+        <v>0.418333333333333</v>
+      </c>
+      <c r="C13">
+        <v>0.391666666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>650</v>
+      </c>
+      <c r="B14">
+        <v>0.39692307692307699</v>
+      </c>
+      <c r="C14">
+        <v>0.395384615384615</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>700</v>
+      </c>
+      <c r="B15">
+        <v>0.39</v>
+      </c>
+      <c r="C15">
+        <v>0.40285714285714302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>750</v>
+      </c>
+      <c r="B16">
+        <v>0.398666666666667</v>
+      </c>
+      <c r="C16">
+        <v>0.38533333333333297</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>800</v>
+      </c>
+      <c r="B17">
+        <v>0.40125</v>
+      </c>
+      <c r="C17">
+        <v>0.37874999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>850</v>
+      </c>
+      <c r="B18">
+        <v>0.41529411764705898</v>
+      </c>
+      <c r="C18">
+        <v>0.42941176470588199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>900</v>
+      </c>
+      <c r="B19">
+        <v>0.41222222222222199</v>
+      </c>
+      <c r="C19">
+        <v>0.43888888888888899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>950</v>
+      </c>
+      <c r="B20">
+        <v>0.35368421052631599</v>
+      </c>
+      <c r="C20">
+        <v>0.35368421052631599</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1000</v>
+      </c>
+      <c r="B21">
+        <v>0.35</v>
+      </c>
+      <c r="C21">
+        <v>0.38900000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>